<commit_message>
novy neterm a opraveni chyb
</commit_message>
<xml_diff>
--- a/ifj21_grammar.xlsx
+++ b/ifj21_grammar.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kuba\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ifj21\IFJ21\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECCF2410-B036-4050-8253-2431730A6974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{416895E0-0094-4F8F-A13F-FE86F2067039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{5A4454C4-5F12-487B-9D4F-E9A3515B76C3}"/>
+    <workbookView xWindow="19395" yWindow="1110" windowWidth="11175" windowHeight="13710" xr2:uid="{5A4454C4-5F12-487B-9D4F-E9A3515B76C3}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="46">
   <si>
     <t>&lt;program&gt;</t>
   </si>
@@ -48,9 +48,6 @@
     <t>require</t>
   </si>
   <si>
-    <t>"ifj21'</t>
-  </si>
-  <si>
     <t>global</t>
   </si>
   <si>
@@ -144,9 +141,6 @@
     <t>if</t>
   </si>
   <si>
-    <t>&lt;cond&gt;</t>
-  </si>
-  <si>
     <t>then</t>
   </si>
   <si>
@@ -171,7 +165,13 @@
     <t>number</t>
   </si>
   <si>
-    <t>a</t>
+    <t>&lt;ID_assign_or_fun&gt;</t>
+  </si>
+  <si>
+    <t>term</t>
+  </si>
+  <si>
+    <t>"ifj21"</t>
   </si>
 </sst>
 </file>
@@ -524,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F9BCA8C-A81E-427A-AC13-57687CE7E23F}">
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,7 +552,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -566,456 +566,455 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>8</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>9</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>10</v>
       </c>
-      <c r="H3" t="s">
-        <v>11</v>
-      </c>
       <c r="I3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
       <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
         <v>12</v>
       </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>13</v>
-      </c>
-      <c r="I4" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
         <v>18</v>
-      </c>
-      <c r="C8" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
         <v>19</v>
       </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
       <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
         <v>18</v>
-      </c>
-      <c r="D10" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
         <v>6</v>
       </c>
-      <c r="C16" t="s">
-        <v>7</v>
-      </c>
       <c r="D16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
         <v>6</v>
       </c>
-      <c r="D18" t="s">
-        <v>7</v>
-      </c>
       <c r="E18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" t="s">
+        <v>25</v>
+      </c>
+      <c r="E26" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" t="s">
         <v>30</v>
-      </c>
-      <c r="B26" t="s">
-        <v>25</v>
-      </c>
-      <c r="C26" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" t="s">
-        <v>26</v>
-      </c>
-      <c r="E26" t="s">
-        <v>18</v>
-      </c>
-      <c r="F26" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="C27" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="D27" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E27" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="F27" t="s">
-        <v>34</v>
+        <v>36</v>
+      </c>
+      <c r="G27" t="s">
+        <v>12</v>
+      </c>
+      <c r="H27" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C28" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="D28" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E28" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" t="s">
         <v>13</v>
-      </c>
-      <c r="F28" t="s">
-        <v>38</v>
-      </c>
-      <c r="G28" t="s">
-        <v>13</v>
-      </c>
-      <c r="H28" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>39</v>
+        <v>5</v>
       </c>
       <c r="C29" t="s">
-        <v>36</v>
-      </c>
-      <c r="D29" t="s">
-        <v>40</v>
-      </c>
-      <c r="E29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F29" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="C30" t="s">
         <v>32</v>
       </c>
       <c r="D30" t="s">
-        <v>29</v>
-      </c>
-      <c r="E30" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="B31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32" t="s">
+        <v>28</v>
+      </c>
+      <c r="D32" t="s">
+        <v>32</v>
+      </c>
+      <c r="E32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>30</v>
       </c>
-      <c r="B32" t="s">
-        <v>41</v>
-      </c>
-      <c r="C32" t="s">
-        <v>33</v>
-      </c>
-      <c r="D32" t="s">
-        <v>34</v>
+      <c r="B33" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B34" t="s">
-        <v>29</v>
-      </c>
-      <c r="C34" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B36" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B37" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1023,78 +1022,71 @@
         <v>33</v>
       </c>
       <c r="B38" t="s">
-        <v>45</v>
+        <v>19</v>
+      </c>
+      <c r="C38" t="s">
+        <v>32</v>
+      </c>
+      <c r="D38" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B39" t="s">
         <v>20</v>
-      </c>
-      <c r="C39" t="s">
-        <v>33</v>
-      </c>
-      <c r="D39" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="B40" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="B43" t="s">
-        <v>44</v>
+        <v>19</v>
+      </c>
+      <c r="C43" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B44" t="s">
         <v>20</v>
-      </c>
-      <c r="C44" t="s">
-        <v>6</v>
-      </c>
-      <c r="D44" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>32</v>
-      </c>
-      <c r="B45" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Jakubovy pasti na blbečky
</commit_message>
<xml_diff>
--- a/ifj21_grammar.xlsx
+++ b/ifj21_grammar.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ifj21\IFJ21\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\imstuff\Projects\project\ProjectIFJ21\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{797DB4EF-01CF-46A8-B1E3-EB94D33B1070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9F9F9C9-75CC-489D-9417-4279AB6B103F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32730" yWindow="1605" windowWidth="11175" windowHeight="13710" xr2:uid="{5A4454C4-5F12-487B-9D4F-E9A3515B76C3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5A4454C4-5F12-487B-9D4F-E9A3515B76C3}"/>
   </bookViews>
   <sheets>
-    <sheet name="List1" sheetId="1" r:id="rId1"/>
+    <sheet name="Grammar" sheetId="1" r:id="rId1"/>
+    <sheet name="Table" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="98">
   <si>
     <t>&lt;program&gt;</t>
   </si>
@@ -184,13 +185,157 @@
   </si>
   <si>
     <t>&lt;init&gt;</t>
+  </si>
+  <si>
+    <t>1.</t>
+  </si>
+  <si>
+    <t>2.</t>
+  </si>
+  <si>
+    <t>3.</t>
+  </si>
+  <si>
+    <t>4.</t>
+  </si>
+  <si>
+    <t>5.</t>
+  </si>
+  <si>
+    <t>6.</t>
+  </si>
+  <si>
+    <t>7.</t>
+  </si>
+  <si>
+    <t>8.</t>
+  </si>
+  <si>
+    <t>9.</t>
+  </si>
+  <si>
+    <t>10.</t>
+  </si>
+  <si>
+    <t>11.</t>
+  </si>
+  <si>
+    <t>12.</t>
+  </si>
+  <si>
+    <t>13.</t>
+  </si>
+  <si>
+    <t>14.</t>
+  </si>
+  <si>
+    <t>15.</t>
+  </si>
+  <si>
+    <t>16.</t>
+  </si>
+  <si>
+    <t>17.</t>
+  </si>
+  <si>
+    <t>18.</t>
+  </si>
+  <si>
+    <t>19.</t>
+  </si>
+  <si>
+    <t>20.</t>
+  </si>
+  <si>
+    <t>21.</t>
+  </si>
+  <si>
+    <t>22.</t>
+  </si>
+  <si>
+    <t>23.</t>
+  </si>
+  <si>
+    <t>24.</t>
+  </si>
+  <si>
+    <t>25.</t>
+  </si>
+  <si>
+    <t>26.</t>
+  </si>
+  <si>
+    <t>27.</t>
+  </si>
+  <si>
+    <t>28.</t>
+  </si>
+  <si>
+    <t>29.</t>
+  </si>
+  <si>
+    <t>30.</t>
+  </si>
+  <si>
+    <t>31.</t>
+  </si>
+  <si>
+    <t>32.</t>
+  </si>
+  <si>
+    <t>33.</t>
+  </si>
+  <si>
+    <t>34.</t>
+  </si>
+  <si>
+    <t>35.</t>
+  </si>
+  <si>
+    <t>36.</t>
+  </si>
+  <si>
+    <t>37.</t>
+  </si>
+  <si>
+    <t>38.</t>
+  </si>
+  <si>
+    <t>39.</t>
+  </si>
+  <si>
+    <t>40.</t>
+  </si>
+  <si>
+    <t>41.</t>
+  </si>
+  <si>
+    <t>42.</t>
+  </si>
+  <si>
+    <t>43.</t>
+  </si>
+  <si>
+    <t>44.</t>
+  </si>
+  <si>
+    <t>45.</t>
+  </si>
+  <si>
+    <t>46.</t>
+  </si>
+  <si>
+    <t>47.</t>
+  </si>
+  <si>
+    <t>func</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,16 +359,35 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -231,18 +395,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -557,761 +740,1525 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F9BCA8C-A81E-427A-AC13-57687CE7E23F}">
-  <dimension ref="A1:K49"/>
+  <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" customWidth="1"/>
+    <col min="10" max="10" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>6</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>7</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>8</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>9</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>10</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>14</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>5</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>8</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>11</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>10</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>14</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>12</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>13</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" t="s">
         <v>26</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" t="s">
         <v>5</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>8</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>16</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" t="s">
         <v>17</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" t="s">
         <v>19</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>17</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" t="s">
         <v>6</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>17</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" t="s">
         <v>19</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>17</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" t="s">
         <v>5</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>6</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>17</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="C17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" t="s">
         <v>19</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>5</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>6</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>17</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="C19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="C20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" t="s">
         <v>5</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="C21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="C22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" t="s">
         <v>19</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>5</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="C23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="C24" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" t="s">
         <v>29</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>74</v>
+      </c>
+      <c r="B25" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="C25" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>75</v>
+      </c>
+      <c r="B26" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="C26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" t="s">
         <v>24</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>5</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>25</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>17</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="C27" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" t="s">
         <v>33</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>46</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>34</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>12</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>44</v>
       </c>
-      <c r="H27" t="s">
+      <c r="I27" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B28" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="C28" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" t="s">
         <v>36</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>46</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>37</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>12</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>78</v>
+      </c>
+      <c r="B29" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="C29" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D29" t="s">
         <v>5</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>31</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>28</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B30" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C30" t="s">
+      <c r="C30" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>80</v>
+      </c>
+      <c r="B31" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="C31" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D31" t="s">
         <v>38</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>46</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>81</v>
+      </c>
+      <c r="B32" t="s">
         <v>44</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="C32" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D32" t="s">
         <v>35</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>82</v>
+      </c>
+      <c r="B33" t="s">
         <v>44</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C33" t="s">
+      <c r="C33" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D33" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>83</v>
+      </c>
+      <c r="B34" t="s">
         <v>30</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C34" t="s">
+      <c r="C34" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D34" t="s">
         <v>28</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>84</v>
+      </c>
+      <c r="B35" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C35" t="s">
+      <c r="C35" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D35" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>85</v>
+      </c>
+      <c r="B36" t="s">
         <v>49</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C36" t="s">
+      <c r="C36" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D36" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>86</v>
+      </c>
+      <c r="B37" t="s">
         <v>49</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C37" t="s">
+      <c r="C37" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D37" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>87</v>
+      </c>
+      <c r="B38" t="s">
         <v>48</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C38" t="s">
+      <c r="C38" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D38" t="s">
         <v>46</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>88</v>
+      </c>
+      <c r="B39" t="s">
         <v>48</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C39" t="s">
+      <c r="C39" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D39" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>89</v>
+      </c>
+      <c r="B40" t="s">
         <v>32</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C40" t="s">
+      <c r="C40" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D40" t="s">
         <v>19</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
         <v>46</v>
       </c>
-      <c r="E40" t="s">
+      <c r="F40" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B41" t="s">
         <v>32</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C41" t="s">
+      <c r="C41" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D41" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>91</v>
+      </c>
+      <c r="B42" t="s">
         <v>17</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C42" t="s">
+      <c r="C42" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D42" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>92</v>
+      </c>
+      <c r="B43" t="s">
         <v>17</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C43" t="s">
+      <c r="C43" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D43" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>93</v>
+      </c>
+      <c r="B44" t="s">
         <v>17</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C44" t="s">
+      <c r="C44" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D44" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>94</v>
+      </c>
+      <c r="B45" t="s">
         <v>17</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C45" t="s">
+      <c r="C45" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D45" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>95</v>
+      </c>
+      <c r="B46" t="s">
         <v>31</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C46" t="s">
+      <c r="C46" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D46" t="s">
         <v>19</v>
       </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
         <v>5</v>
       </c>
-      <c r="E46" t="s">
+      <c r="F46" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>96</v>
+      </c>
+      <c r="B47" t="s">
         <v>31</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C47" t="s">
+      <c r="C47" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D47" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A49" s="2" t="s">
+    <row r="49" spans="2:11" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B49" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
-      <c r="G49" s="2"/>
-      <c r="H49" s="2"/>
-      <c r="I49" s="2"/>
-      <c r="J49" s="2"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5"/>
+      <c r="I49" s="5"/>
+      <c r="J49" s="5"/>
+      <c r="K49" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A49:J49"/>
+    <mergeCell ref="B49:K49"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BCD0DCD-2305-4F19-A748-1CF454DD3226}">
+  <dimension ref="A1:R22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X17" sqref="X17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" customWidth="1"/>
+    <col min="5" max="5" width="6.28515625" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" customWidth="1"/>
+    <col min="10" max="10" width="7.85546875" customWidth="1"/>
+    <col min="11" max="11" width="7.5703125" customWidth="1"/>
+    <col min="12" max="13" width="8.28515625" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3">
+        <v>4</v>
+      </c>
+      <c r="E4" s="3">
+        <v>5</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6">
+        <v>7</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3">
+        <v>10</v>
+      </c>
+      <c r="G6" s="3">
+        <v>10</v>
+      </c>
+      <c r="H6" s="3">
+        <v>10</v>
+      </c>
+      <c r="I6" s="3">
+        <v>10</v>
+      </c>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6">
+        <v>10</v>
+      </c>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3">
+        <v>12</v>
+      </c>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6">
+        <v>14</v>
+      </c>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3">
+        <v>16</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6">
+        <v>18</v>
+      </c>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3">
+        <v>20</v>
+      </c>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6">
+        <v>22</v>
+      </c>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3">
+        <v>29</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3">
+        <v>26</v>
+      </c>
+      <c r="M14" s="3">
+        <v>27</v>
+      </c>
+      <c r="N14" s="3">
+        <v>28</v>
+      </c>
+      <c r="O14" s="3">
+        <v>30</v>
+      </c>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6">
+        <v>29</v>
+      </c>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6">
+        <v>26</v>
+      </c>
+      <c r="M15" s="6">
+        <v>27</v>
+      </c>
+      <c r="N15" s="6">
+        <v>28</v>
+      </c>
+      <c r="O15" s="6">
+        <v>30</v>
+      </c>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3">
+        <v>32</v>
+      </c>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="6">
+        <v>34</v>
+      </c>
+      <c r="R17" s="6"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3">
+        <v>7</v>
+      </c>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6">
+        <v>7</v>
+      </c>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3">
+        <v>40</v>
+      </c>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6">
+        <v>42</v>
+      </c>
+      <c r="G21" s="6">
+        <v>43</v>
+      </c>
+      <c r="H21" s="6">
+        <v>44</v>
+      </c>
+      <c r="I21" s="6">
+        <v>45</v>
+      </c>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3">
+        <v>46</v>
+      </c>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>